<commit_message>
25-09-20 Tooltip Estado + Distrito # ynombre.
</commit_message>
<xml_diff>
--- a/data/afiliaciones/26_Sonora.xlsx
+++ b/data/afiliaciones/26_Sonora.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Salamandra/afiliacion/data/afiliaciones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5BCBE9-BA5B-AA4D-B6AF-102910F4D1C6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A310EC-5B96-0F4B-94BC-DDCCCF88E951}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="4320" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10360" yWindow="7940" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="15_Mexico" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="107">
   <si>
     <t>id</t>
   </si>
@@ -326,6 +326,21 @@
   </si>
   <si>
     <t>Sonora</t>
+  </si>
+  <si>
+    <t>SAN LUIS RIO COLORADO</t>
+  </si>
+  <si>
+    <t>NOGALES</t>
+  </si>
+  <si>
+    <t>HERMOSILLO</t>
+  </si>
+  <si>
+    <t>GUAYMAS</t>
+  </si>
+  <si>
+    <t>CD. OBREGON</t>
   </si>
 </sst>
 </file>
@@ -1166,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1259,7 +1274,16 @@
         <v>101</v>
       </c>
       <c r="J2">
-        <v>2601</v>
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>102</v>
       </c>
       <c r="O2" t="s">
         <v>30</v>
@@ -1297,7 +1321,16 @@
         <v>101</v>
       </c>
       <c r="J3">
-        <v>2601</v>
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>102</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>102</v>
       </c>
       <c r="O3" t="s">
         <v>20</v>
@@ -1335,7 +1368,16 @@
         <v>101</v>
       </c>
       <c r="J4">
-        <v>2601</v>
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>102</v>
       </c>
       <c r="O4" t="s">
         <v>30</v>
@@ -1373,7 +1415,16 @@
         <v>101</v>
       </c>
       <c r="J5">
-        <v>2601</v>
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>102</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>102</v>
       </c>
       <c r="O5" t="s">
         <v>30</v>
@@ -1411,7 +1462,16 @@
         <v>101</v>
       </c>
       <c r="J6">
-        <v>2601</v>
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>102</v>
       </c>
       <c r="O6" t="s">
         <v>39</v>
@@ -1449,7 +1509,16 @@
         <v>101</v>
       </c>
       <c r="J7">
-        <v>2602</v>
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>103</v>
       </c>
       <c r="O7" t="s">
         <v>30</v>
@@ -1487,7 +1556,16 @@
         <v>101</v>
       </c>
       <c r="J8">
-        <v>2602</v>
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>103</v>
       </c>
       <c r="O8" t="s">
         <v>30</v>
@@ -1525,7 +1603,16 @@
         <v>101</v>
       </c>
       <c r="J9">
-        <v>2602</v>
+        <v>2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9" t="s">
+        <v>103</v>
       </c>
       <c r="O9" t="s">
         <v>30</v>
@@ -1563,7 +1650,16 @@
         <v>101</v>
       </c>
       <c r="J10">
-        <v>2602</v>
+        <v>2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>103</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>103</v>
       </c>
       <c r="O10" t="s">
         <v>20</v>
@@ -1601,7 +1697,16 @@
         <v>101</v>
       </c>
       <c r="J11">
-        <v>2602</v>
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>103</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>103</v>
       </c>
       <c r="O11" t="s">
         <v>30</v>
@@ -1639,7 +1744,16 @@
         <v>101</v>
       </c>
       <c r="J12">
-        <v>2602</v>
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>103</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>103</v>
       </c>
       <c r="O12" t="s">
         <v>39</v>
@@ -1677,7 +1791,16 @@
         <v>101</v>
       </c>
       <c r="J13">
-        <v>2602</v>
+        <v>2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>103</v>
       </c>
       <c r="O13" t="s">
         <v>39</v>
@@ -1715,7 +1838,16 @@
         <v>101</v>
       </c>
       <c r="J14">
-        <v>2602</v>
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>103</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>103</v>
       </c>
       <c r="O14" t="s">
         <v>30</v>
@@ -1753,7 +1885,16 @@
         <v>101</v>
       </c>
       <c r="J15">
-        <v>2603</v>
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>104</v>
+      </c>
+      <c r="L15">
+        <v>3</v>
+      </c>
+      <c r="M15" t="s">
+        <v>104</v>
       </c>
       <c r="O15" t="s">
         <v>39</v>
@@ -1791,7 +1932,16 @@
         <v>101</v>
       </c>
       <c r="J16">
-        <v>2603</v>
+        <v>3</v>
+      </c>
+      <c r="K16" t="s">
+        <v>104</v>
+      </c>
+      <c r="L16">
+        <v>3</v>
+      </c>
+      <c r="M16" t="s">
+        <v>104</v>
       </c>
       <c r="O16" t="s">
         <v>39</v>
@@ -1829,7 +1979,16 @@
         <v>101</v>
       </c>
       <c r="J17">
-        <v>2603</v>
+        <v>3</v>
+      </c>
+      <c r="K17" t="s">
+        <v>104</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17" t="s">
+        <v>104</v>
       </c>
       <c r="O17" t="s">
         <v>30</v>
@@ -1867,7 +2026,16 @@
         <v>101</v>
       </c>
       <c r="J18">
-        <v>2603</v>
+        <v>3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>104</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18" t="s">
+        <v>104</v>
       </c>
       <c r="O18" t="s">
         <v>20</v>
@@ -1905,7 +2073,16 @@
         <v>101</v>
       </c>
       <c r="J19">
-        <v>2603</v>
+        <v>3</v>
+      </c>
+      <c r="K19" t="s">
+        <v>104</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19" t="s">
+        <v>104</v>
       </c>
       <c r="O19" t="s">
         <v>30</v>
@@ -1943,7 +2120,16 @@
         <v>101</v>
       </c>
       <c r="J20">
-        <v>2603</v>
+        <v>3</v>
+      </c>
+      <c r="K20" t="s">
+        <v>104</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20" t="s">
+        <v>104</v>
       </c>
       <c r="O20" t="s">
         <v>30</v>
@@ -1981,12 +2167,961 @@
         <v>101</v>
       </c>
       <c r="J21">
-        <v>2603</v>
+        <v>3</v>
+      </c>
+      <c r="K21" t="s">
+        <v>104</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
+      </c>
+      <c r="M21" t="s">
+        <v>104</v>
       </c>
       <c r="O21" t="s">
         <v>39</v>
       </c>
       <c r="P21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22">
+        <v>5525451487</v>
+      </c>
+      <c r="H22">
+        <v>26</v>
+      </c>
+      <c r="I22" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22" t="s">
+        <v>105</v>
+      </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
+      <c r="M22" t="s">
+        <v>105</v>
+      </c>
+      <c r="O22" t="s">
+        <v>30</v>
+      </c>
+      <c r="P22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23">
+        <v>5536214589</v>
+      </c>
+      <c r="H23">
+        <v>26</v>
+      </c>
+      <c r="I23" t="s">
+        <v>101</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23" t="s">
+        <v>105</v>
+      </c>
+      <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="M23" t="s">
+        <v>105</v>
+      </c>
+      <c r="O23" t="s">
+        <v>20</v>
+      </c>
+      <c r="P23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24">
+        <v>5514789632</v>
+      </c>
+      <c r="H24">
+        <v>26</v>
+      </c>
+      <c r="I24" t="s">
+        <v>101</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>105</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24" t="s">
+        <v>105</v>
+      </c>
+      <c r="O24" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>60</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25">
+        <v>5563258941</v>
+      </c>
+      <c r="H25">
+        <v>26</v>
+      </c>
+      <c r="I25" t="s">
+        <v>101</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25" t="s">
+        <v>105</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25" t="s">
+        <v>105</v>
+      </c>
+      <c r="O25" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26">
+        <v>5547896321</v>
+      </c>
+      <c r="H26">
+        <v>26</v>
+      </c>
+      <c r="I26" t="s">
+        <v>101</v>
+      </c>
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="K26" t="s">
+        <v>104</v>
+      </c>
+      <c r="L26">
+        <v>5</v>
+      </c>
+      <c r="M26" t="s">
+        <v>104</v>
+      </c>
+      <c r="O26" t="s">
+        <v>39</v>
+      </c>
+      <c r="P26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27">
+        <v>5589632541</v>
+      </c>
+      <c r="H27">
+        <v>26</v>
+      </c>
+      <c r="I27" t="s">
+        <v>101</v>
+      </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
+      <c r="K27" t="s">
+        <v>104</v>
+      </c>
+      <c r="L27">
+        <v>5</v>
+      </c>
+      <c r="M27" t="s">
+        <v>104</v>
+      </c>
+      <c r="O27" t="s">
+        <v>30</v>
+      </c>
+      <c r="P27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28">
+        <v>33</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28">
+        <v>5532145698</v>
+      </c>
+      <c r="H28">
+        <v>26</v>
+      </c>
+      <c r="I28" t="s">
+        <v>101</v>
+      </c>
+      <c r="J28">
+        <v>5</v>
+      </c>
+      <c r="K28" t="s">
+        <v>104</v>
+      </c>
+      <c r="L28">
+        <v>5</v>
+      </c>
+      <c r="M28" t="s">
+        <v>104</v>
+      </c>
+      <c r="O28" t="s">
+        <v>30</v>
+      </c>
+      <c r="P28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29">
+        <v>47</v>
+      </c>
+      <c r="E29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29">
+        <v>5578945612</v>
+      </c>
+      <c r="H29">
+        <v>26</v>
+      </c>
+      <c r="I29" t="s">
+        <v>101</v>
+      </c>
+      <c r="J29">
+        <v>5</v>
+      </c>
+      <c r="K29" t="s">
+        <v>104</v>
+      </c>
+      <c r="L29">
+        <v>5</v>
+      </c>
+      <c r="M29" t="s">
+        <v>104</v>
+      </c>
+      <c r="O29" t="s">
+        <v>30</v>
+      </c>
+      <c r="P29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30">
+        <v>5565412398</v>
+      </c>
+      <c r="H30">
+        <v>26</v>
+      </c>
+      <c r="I30" t="s">
+        <v>101</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
+      </c>
+      <c r="K30" t="s">
+        <v>104</v>
+      </c>
+      <c r="L30">
+        <v>5</v>
+      </c>
+      <c r="M30" t="s">
+        <v>104</v>
+      </c>
+      <c r="O30" t="s">
+        <v>20</v>
+      </c>
+      <c r="P30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31">
+        <v>38</v>
+      </c>
+      <c r="E31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31">
+        <v>5541236589</v>
+      </c>
+      <c r="H31">
+        <v>26</v>
+      </c>
+      <c r="I31" t="s">
+        <v>101</v>
+      </c>
+      <c r="J31">
+        <v>5</v>
+      </c>
+      <c r="K31" t="s">
+        <v>104</v>
+      </c>
+      <c r="L31">
+        <v>5</v>
+      </c>
+      <c r="M31" t="s">
+        <v>104</v>
+      </c>
+      <c r="O31" t="s">
+        <v>30</v>
+      </c>
+      <c r="P31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32">
+        <v>5598741236</v>
+      </c>
+      <c r="H32">
+        <v>26</v>
+      </c>
+      <c r="I32" t="s">
+        <v>101</v>
+      </c>
+      <c r="J32">
+        <v>6</v>
+      </c>
+      <c r="K32" t="s">
+        <v>106</v>
+      </c>
+      <c r="L32">
+        <v>6</v>
+      </c>
+      <c r="M32" t="s">
+        <v>106</v>
+      </c>
+      <c r="O32" t="s">
+        <v>39</v>
+      </c>
+      <c r="P32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33">
+        <v>44</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33">
+        <v>5536987412</v>
+      </c>
+      <c r="H33">
+        <v>26</v>
+      </c>
+      <c r="I33" t="s">
+        <v>101</v>
+      </c>
+      <c r="J33">
+        <v>6</v>
+      </c>
+      <c r="K33" t="s">
+        <v>106</v>
+      </c>
+      <c r="L33">
+        <v>6</v>
+      </c>
+      <c r="M33" t="s">
+        <v>106</v>
+      </c>
+      <c r="O33" t="s">
+        <v>39</v>
+      </c>
+      <c r="P33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34">
+        <v>52</v>
+      </c>
+      <c r="E34" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34">
+        <v>5574125896</v>
+      </c>
+      <c r="H34">
+        <v>26</v>
+      </c>
+      <c r="I34" t="s">
+        <v>101</v>
+      </c>
+      <c r="J34">
+        <v>6</v>
+      </c>
+      <c r="K34" t="s">
+        <v>106</v>
+      </c>
+      <c r="L34">
+        <v>6</v>
+      </c>
+      <c r="M34" t="s">
+        <v>106</v>
+      </c>
+      <c r="O34" t="s">
+        <v>30</v>
+      </c>
+      <c r="P34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35">
+        <v>31</v>
+      </c>
+      <c r="E35" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" t="s">
+        <v>75</v>
+      </c>
+      <c r="G35">
+        <v>5525874136</v>
+      </c>
+      <c r="H35">
+        <v>26</v>
+      </c>
+      <c r="I35" t="s">
+        <v>101</v>
+      </c>
+      <c r="J35">
+        <v>6</v>
+      </c>
+      <c r="K35" t="s">
+        <v>106</v>
+      </c>
+      <c r="L35">
+        <v>6</v>
+      </c>
+      <c r="M35" t="s">
+        <v>106</v>
+      </c>
+      <c r="O35" t="s">
+        <v>39</v>
+      </c>
+      <c r="P35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36">
+        <v>40</v>
+      </c>
+      <c r="E36" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36">
+        <v>5587456321</v>
+      </c>
+      <c r="H36">
+        <v>26</v>
+      </c>
+      <c r="I36" t="s">
+        <v>101</v>
+      </c>
+      <c r="J36">
+        <v>6</v>
+      </c>
+      <c r="K36" t="s">
+        <v>106</v>
+      </c>
+      <c r="L36">
+        <v>6</v>
+      </c>
+      <c r="M36" t="s">
+        <v>106</v>
+      </c>
+      <c r="O36" t="s">
+        <v>39</v>
+      </c>
+      <c r="P36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37">
+        <v>58</v>
+      </c>
+      <c r="E37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37">
+        <v>5532569874</v>
+      </c>
+      <c r="H37">
+        <v>26</v>
+      </c>
+      <c r="I37" t="s">
+        <v>101</v>
+      </c>
+      <c r="J37">
+        <v>7</v>
+      </c>
+      <c r="K37" t="s">
+        <v>106</v>
+      </c>
+      <c r="L37">
+        <v>7</v>
+      </c>
+      <c r="M37" t="s">
+        <v>106</v>
+      </c>
+      <c r="O37" t="s">
+        <v>30</v>
+      </c>
+      <c r="P37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38">
+        <v>36</v>
+      </c>
+      <c r="E38" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" t="s">
+        <v>87</v>
+      </c>
+      <c r="G38">
+        <v>5563258741</v>
+      </c>
+      <c r="H38">
+        <v>26</v>
+      </c>
+      <c r="I38" t="s">
+        <v>101</v>
+      </c>
+      <c r="J38">
+        <v>7</v>
+      </c>
+      <c r="K38" t="s">
+        <v>106</v>
+      </c>
+      <c r="L38">
+        <v>7</v>
+      </c>
+      <c r="M38" t="s">
+        <v>106</v>
+      </c>
+      <c r="O38" t="s">
+        <v>20</v>
+      </c>
+      <c r="P38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39">
+        <v>49</v>
+      </c>
+      <c r="E39" t="s">
+        <v>90</v>
+      </c>
+      <c r="F39" t="s">
+        <v>91</v>
+      </c>
+      <c r="G39">
+        <v>5547893216</v>
+      </c>
+      <c r="H39">
+        <v>26</v>
+      </c>
+      <c r="I39" t="s">
+        <v>101</v>
+      </c>
+      <c r="J39">
+        <v>7</v>
+      </c>
+      <c r="K39" t="s">
+        <v>106</v>
+      </c>
+      <c r="L39">
+        <v>7</v>
+      </c>
+      <c r="M39" t="s">
+        <v>106</v>
+      </c>
+      <c r="O39" t="s">
+        <v>30</v>
+      </c>
+      <c r="P39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40">
+        <v>30</v>
+      </c>
+      <c r="E40" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" t="s">
+        <v>95</v>
+      </c>
+      <c r="G40">
+        <v>5578963214</v>
+      </c>
+      <c r="H40">
+        <v>26</v>
+      </c>
+      <c r="I40" t="s">
+        <v>101</v>
+      </c>
+      <c r="J40">
+        <v>7</v>
+      </c>
+      <c r="K40" t="s">
+        <v>106</v>
+      </c>
+      <c r="L40">
+        <v>7</v>
+      </c>
+      <c r="M40" t="s">
+        <v>106</v>
+      </c>
+      <c r="O40" t="s">
+        <v>30</v>
+      </c>
+      <c r="P40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41">
+        <v>53</v>
+      </c>
+      <c r="E41" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" t="s">
+        <v>99</v>
+      </c>
+      <c r="G41">
+        <v>5514789632</v>
+      </c>
+      <c r="H41">
+        <v>26</v>
+      </c>
+      <c r="I41" t="s">
+        <v>101</v>
+      </c>
+      <c r="J41">
+        <v>7</v>
+      </c>
+      <c r="K41" t="s">
+        <v>106</v>
+      </c>
+      <c r="L41">
+        <v>7</v>
+      </c>
+      <c r="M41" t="s">
+        <v>106</v>
+      </c>
+      <c r="O41" t="s">
+        <v>39</v>
+      </c>
+      <c r="P41" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>